<commit_message>
Move review package to annotation_process
</commit_message>
<xml_diff>
--- a/sample_data/annotation/8141_annotation_labels.xlsx
+++ b/sample_data/annotation/8141_annotation_labels.xlsx
@@ -1013,22 +1013,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>Lage_Gelaende_Planzeichen</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>AnFluchtlinie</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Strassen_und_Gehsteige</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>GehsteigbreiteMin</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Lage_Gelaende_Planzeichen</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>AnFluchtlinie</t>
         </is>
       </c>
     </row>
@@ -1099,22 +1099,22 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>Flaeche</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Flaechen</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Dach</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>BegruenungDach</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Flaeche</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Flaechen</t>
         </is>
       </c>
     </row>
@@ -1158,37 +1158,37 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>Dachart</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Ausgestaltung_und_Sonstiges</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>GebaeudeBautyp</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Flaeche</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Flaechen</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Dach</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
           <t>BegruenungDach</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Ausgestaltung_und_Sonstiges</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>GebaeudeBautyp</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Dach</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Dachart</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Flaeche</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Flaechen</t>
         </is>
       </c>
     </row>
@@ -1305,42 +1305,42 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>Lage_Gelaende_Planzeichen</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Planzeichen</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>Dach</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Dachart</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Flaeche</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Flaechen</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Dach</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
         <is>
           <t>BegruenungDach</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Lage_Gelaende_Planzeichen</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Planzeichen</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Dach</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Dachart</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>Flaeche</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Flaechen</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fill header for review
</commit_message>
<xml_diff>
--- a/sample_data/annotation/8141_annotation_labels.xlsx
+++ b/sample_data/annotation/8141_annotation_labels.xlsx
@@ -1013,22 +1013,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>Strassen_und_Gehsteige</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>GehsteigbreiteMin</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Lage_Gelaende_Planzeichen</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>AnFluchtlinie</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Strassen_und_Gehsteige</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>GehsteigbreiteMin</t>
         </is>
       </c>
     </row>
@@ -1089,22 +1089,22 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>Flaeche</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Flaechen</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>Dach</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>DachneigungMax</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Flaeche</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Flaechen</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1153,42 +1153,42 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>Flaeche</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Flaechen</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>Dach</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>Dachart</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Dach</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>BegruenungDach</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>Ausgestaltung_und_Sonstiges</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>GebaeudeBautyp</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Flaeche</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Flaechen</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Dach</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>BegruenungDach</t>
         </is>
       </c>
     </row>
@@ -1273,22 +1273,22 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>Ausgestaltung_und_Sonstiges</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>UnterbrechungGeschlosseneBauweise</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>Lage_Gelaende_Planzeichen</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>Planzeichen</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Ausgestaltung_und_Sonstiges</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>UnterbrechungGeschlosseneBauweise</t>
         </is>
       </c>
     </row>
@@ -1305,42 +1305,42 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>Flaeche</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Flaechen</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Dach</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Dachart</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Dach</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>BegruenungDach</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
           <t>Lage_Gelaende_Planzeichen</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>Planzeichen</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Dach</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Dachart</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Flaeche</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Flaechen</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>Dach</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>BegruenungDach</t>
         </is>
       </c>
     </row>

</xml_diff>